<commit_message>
Parts Order and Pressure Accuracy Table
</commit_message>
<xml_diff>
--- a/PressureTable.xlsx
+++ b/PressureTable.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Goal Pressure</t>
   </si>
@@ -33,6 +33,12 @@
   </si>
   <si>
     <t>Pressure Sensor</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>Percent Error</t>
   </si>
 </sst>
 </file>
@@ -101,11 +107,72 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Pressure Sensor Reading Versus Actual Tire Pressure</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.7369730011911239E-2"/>
+          <c:y val="9.1919761556476923E-2"/>
+          <c:w val="0.79418003617487465"/>
+          <c:h val="0.79243986268078903"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -114,36 +181,238 @@
             <c:v>Actual Pressure</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="bg2">
+                <a:lumMod val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
               <a:noFill/>
-              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.1564535755775487E-2"/>
+                  <c:y val="-3.436489864906881E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.3842371843889239E-2"/>
+                  <c:y val="-2.9270980025822652E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.6718472418021983E-2"/>
+                  <c:y val="-3.1817939337445637E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.0087041196711908E-2"/>
+                  <c:y val="-3.4364898649068713E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.6563414481714039E-2"/>
+                  <c:y val="-3.6911857960691886E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.7168971405673386E-2"/>
+                  <c:y val="-2.163010209095332E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.1546076092231224E-2"/>
+                  <c:y val="-2.9270980025822558E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.4464145883269961E-2"/>
+                  <c:y val="-1.2544275979686896E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-          </c:marker>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:errBars>
-            <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
             <c:val val="10"/>
             <c:spPr>
               <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:ln w="19050">
                 <a:solidFill>
                   <a:srgbClr val="FF0000"/>
                 </a:solidFill>
@@ -152,7 +421,7 @@
               <a:effectLst/>
             </c:spPr>
           </c:errBars>
-          <c:xVal>
+          <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$2:$I$2</c:f>
               <c:numCache>
@@ -184,8 +453,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
               <c:f>Sheet1!$B$3:$I$3</c:f>
               <c:numCache>
@@ -195,30 +464,29 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.8000000000000007</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.8</c:v>
+                  <c:v>20.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.3</c:v>
+                  <c:v>30.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>49.8</c:v>
+                  <c:v>50.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60.7</c:v>
+                  <c:v>60.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70.2</c:v>
+                  <c:v>70.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
+          </c:val>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -227,28 +495,229 @@
             <c:v>Pressure Sensor</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:ln>
               <a:noFill/>
-              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="diamond"/>
-            <c:size val="7"/>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.5606636839551195E-3"/>
+                  <c:y val="-2.4177061402576493E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.5797437245415647E-3"/>
+                  <c:y val="-3.181793933744554E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="6.664832834760284E-4"/>
+                  <c:y val="-2.9270980025822558E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.4473083908063419E-3"/>
+                  <c:y val="-3.6911857960691796E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.0056504945615422E-3"/>
+                  <c:y val="-2.6724020714199478E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.4646467802891051E-3"/>
+                  <c:y val="-2.1630102090953274E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.5292385997676571E-3"/>
+                  <c:y val="-3.1817939337445637E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.9236816758084206E-3"/>
+                  <c:y val="-6.492841038854566E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="00B050"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-          </c:marker>
-          <c:xVal>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$2:$I$2</c:f>
               <c:numCache>
@@ -280,74 +749,111 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
               <c:f>Sheet1!$B$4:$I$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.056</c:v>
+                  <c:v>1.08</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.6999999999999993</c:v>
+                  <c:v>11.02</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.2</c:v>
+                  <c:v>20.84</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.1</c:v>
+                  <c:v>30.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>40.520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>51.43</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60.2</c:v>
+                  <c:v>60.48</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>65</c:v>
+                  <c:v>69.83</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
+          </c:val>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="400441440"/>
-        <c:axId val="400437520"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="400441440"/>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="316056904"/>
+        <c:axId val="316060040"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="316056904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Target Pressure (psi)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -355,12 +861,7 @@
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
+            <a:noFill/>
             <a:round/>
           </a:ln>
           <a:effectLst/>
@@ -370,12 +871,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx2"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -385,12 +883,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="400437520"/>
+        <c:crossAx val="316060040"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="400437520"/>
+        <c:axId val="316060040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -401,7 +902,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="tx2">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
@@ -411,20 +912,64 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Pressure Ranges (psi)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -433,12 +978,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx2"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -448,9 +990,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="400441440"/>
+        <c:crossAx val="316056904"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -460,6 +1002,44 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.85366961225916627"/>
+          <c:y val="0.43998702053490957"/>
+          <c:w val="0.14564476383683481"/>
+          <c:h val="0.13467077442403624"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -470,7 +1050,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="tx2">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -494,6 +1074,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -538,35 +1119,29 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -579,7 +1154,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -587,7 +1162,7 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -595,17 +1170,14 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
@@ -614,9 +1186,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
@@ -639,35 +1210,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="31750" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -676,33 +1247,32 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="12700">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="lt2"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -718,21 +1288,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -742,23 +1307,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -767,17 +1331,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -786,14 +1350,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -805,26 +1369,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -838,17 +1396,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -857,17 +1414,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -876,17 +1433,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -895,27 +1451,24 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -923,132 +1476,113 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1086,6 +1620,63 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.88014</cdr:x>
+      <cdr:y>0.57784</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.99726</cdr:x>
+      <cdr:y>0.78558</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="7649766" y="2881314"/>
+          <a:ext cx="1017985" cy="1035843"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>*Red</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> bar indicates contraint range of +- 10 psi.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1351,10 +1942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I7"/>
+  <dimension ref="A2:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="I7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1399,25 +1990,25 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>9.8000000000000007</v>
+        <v>10</v>
       </c>
       <c r="D3">
-        <v>19.8</v>
+        <v>20.5</v>
       </c>
       <c r="E3">
-        <v>30.3</v>
+        <v>30.5</v>
       </c>
       <c r="F3">
         <v>40</v>
       </c>
       <c r="G3">
-        <v>49.8</v>
+        <v>50.5</v>
       </c>
       <c r="H3">
-        <v>60.7</v>
+        <v>60.5</v>
       </c>
       <c r="I3">
-        <v>70.2</v>
+        <v>70.5</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1425,51 +2016,102 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1.056</v>
+        <v>1.08</v>
       </c>
       <c r="C4">
-        <v>9.6999999999999993</v>
+        <v>11.02</v>
       </c>
       <c r="D4">
-        <v>20.2</v>
+        <v>20.84</v>
       </c>
       <c r="E4">
-        <v>30.1</v>
+        <v>30.7</v>
       </c>
       <c r="F4">
-        <v>40</v>
+        <v>40.520000000000003</v>
       </c>
       <c r="G4">
-        <v>50</v>
+        <v>51.43</v>
       </c>
       <c r="H4">
-        <v>60.2</v>
+        <v>60.48</v>
       </c>
       <c r="I4">
-        <v>65</v>
+        <v>69.83</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>10</v>
-      </c>
-      <c r="E7">
-        <v>20</v>
-      </c>
-      <c r="F7">
-        <v>30</v>
-      </c>
-      <c r="G7">
-        <v>40</v>
-      </c>
-      <c r="H7">
-        <v>50</v>
-      </c>
-      <c r="I7">
-        <v>60</v>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <f>ABS(B3-B4)</f>
+        <v>1.08</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:I5" si="0">ABS(C3-C4)</f>
+        <v>1.0199999999999996</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.33999999999999986</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.19999999999999929</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0.52000000000000313</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>0.92999999999999972</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>2.0000000000003126E-2</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>0.67000000000000171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="e">
+        <f t="shared" ref="B6:C6" si="1">((B5)/B3)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>10.199999999999996</v>
+      </c>
+      <c r="D6">
+        <f>((D5)/D3)*100</f>
+        <v>1.6585365853658531</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:I6" si="2">((E5)/E3)*100</f>
+        <v>0.65573770491803041</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>1.3000000000000078</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>1.8415841584158412</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="2"/>
+        <v>3.3057851239674592E-2</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>0.9503546099290805</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Newer Version of Main Code
</commit_message>
<xml_diff>
--- a/PressureTable.xlsx
+++ b/PressureTable.xlsx
@@ -806,11 +806,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="320474336"/>
-        <c:axId val="320475120"/>
+        <c:axId val="319463688"/>
+        <c:axId val="319464472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="320474336"/>
+        <c:axId val="319463688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -899,7 +899,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="320475120"/>
+        <c:crossAx val="319464472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -907,7 +907,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="320475120"/>
+        <c:axId val="319464472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="80"/>
@@ -1011,7 +1011,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="320474336"/>
+        <c:crossAx val="319463688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1710,7 +1710,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> contraint range of </a:t>
+            <a:t> constraint range of </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="0" i="0" baseline="0">

</xml_diff>